<commit_message>
Added functionality for rendering images. More graphics.
</commit_message>
<xml_diff>
--- a/Assets/images/ProjectImageMap.xlsx
+++ b/Assets/images/ProjectImageMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Game Object</t>
   </si>
@@ -41,15 +41,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Bet1Button</t>
-  </si>
-  <si>
-    <t>Bet10Button</t>
-  </si>
-  <si>
-    <t>Bet100Button</t>
-  </si>
-  <si>
     <t>Reel 1</t>
   </si>
   <si>
@@ -60,6 +51,39 @@
   </si>
   <si>
     <t>HitmonSpin</t>
+  </si>
+  <si>
+    <t>Bet1</t>
+  </si>
+  <si>
+    <t>Bet10</t>
+  </si>
+  <si>
+    <t>Bet100</t>
+  </si>
+  <si>
+    <t>Raikou</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>Magikarp</t>
+  </si>
+  <si>
+    <t>Charizard</t>
+  </si>
+  <si>
+    <t>Articuno</t>
+  </si>
+  <si>
+    <t>Voltorb</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Jigglypuff</t>
   </si>
 </sst>
 </file>
@@ -129,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -139,6 +163,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,11 +450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -432,7 +463,7 @@
     <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -449,62 +480,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4">
-        <v>64</v>
-      </c>
-      <c r="C2" s="4">
-        <v>64</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5">
+        <v>60</v>
       </c>
       <c r="D2" s="4">
         <v>168</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>382</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4">
-        <v>64</v>
-      </c>
-      <c r="C3" s="4">
-        <v>64</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5">
+        <v>60</v>
       </c>
       <c r="D3" s="4">
         <f>D2+64+8</f>
         <v>240</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>382</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>64</v>
-      </c>
-      <c r="C4" s="4">
-        <v>64</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5">
+        <v>60</v>
       </c>
       <c r="D4" s="4">
         <f>D3+64+8</f>
         <v>312</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>70</v>
@@ -512,16 +543,16 @@
       <c r="C5" s="2">
         <v>70</v>
       </c>
-      <c r="D5" s="4">
-        <v>402</v>
-      </c>
-      <c r="E5" s="4">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="D5" s="5">
+        <v>380</v>
+      </c>
+      <c r="E5" s="5">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>67</v>
@@ -535,10 +566,18 @@
       <c r="E6" s="2">
         <v>210</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F6" s="7">
+        <f>FLOOR((D6+((B6-$B$9)/2)),1)</f>
+        <v>193</v>
+      </c>
+      <c r="G6" s="1">
+        <f>E6+7</f>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>67</v>
@@ -552,10 +591,22 @@
       <c r="E7" s="2">
         <v>210</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="F7" s="7">
+        <f t="shared" ref="F7:F8" si="0">FLOOR((D7+((B7-$B$9)/2)),1)</f>
+        <v>273</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ref="G7:G8" si="1">E7+7</f>
+        <v>217</v>
+      </c>
+      <c r="I7" s="7">
+        <f>F7-F6</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>67</v>
@@ -569,8 +620,119 @@
       <c r="E8" s="2">
         <v>210</v>
       </c>
+      <c r="F8" s="7">
+        <f t="shared" si="0"/>
+        <v>351</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>217</v>
+      </c>
+      <c r="I8" s="7">
+        <f>F8-F7</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>